<commit_message>
add training phrases and modify entities
</commit_message>
<xml_diff>
--- a/src/Training Phrases.xlsx
+++ b/src/Training Phrases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="202">
   <si>
     <t>Phrase</t>
   </si>
@@ -49,7 +49,7 @@
     <t>tell me about the director of Mine 9.</t>
   </si>
   <si>
-    <t>what is actors of Joker.</t>
+    <t>who are actors of Joker.</t>
   </si>
   <si>
     <t>actors</t>
@@ -277,13 +277,13 @@
     <t>the hyperlink of First Cow.</t>
   </si>
   <si>
-    <t>Recommend some comedy to watch.</t>
+    <t>Recommend some comedy to watch</t>
   </si>
   <si>
     <t>recom_keyword</t>
   </si>
   <si>
-    <t>I want to watch a comedy.</t>
+    <t>I want to watch a comedy</t>
   </si>
   <si>
     <t>Could you recommend some comedy?</t>
@@ -292,37 +292,64 @@
     <t>Could you recommend some comedy to me?</t>
   </si>
   <si>
-    <t>I would like to watch a comedy.</t>
-  </si>
-  <si>
-    <t>List some popular comedy.</t>
-  </si>
-  <si>
-    <t>Suggest some comedy.</t>
-  </si>
-  <si>
-    <t>Recommend some interesting movie to watch</t>
-  </si>
-  <si>
-    <t>I want to watch a happy film</t>
+    <t xml:space="preserve">I want to watch a comedy. Any recommendations? </t>
+  </si>
+  <si>
+    <t>I would like to watch a comedy</t>
+  </si>
+  <si>
+    <t>List some popular comedy</t>
+  </si>
+  <si>
+    <t>Suggest some comedy</t>
+  </si>
+  <si>
+    <t>Recommend some horror movie to watch</t>
   </si>
   <si>
     <t>Could you recommend some horror movies?</t>
   </si>
   <si>
-    <t>Could you recommend some action films to me?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I want to watch a blue movie. Any recommendations? </t>
-  </si>
-  <si>
-    <t>I would like to watch a sad film</t>
-  </si>
-  <si>
-    <t>List some popular romantic movies</t>
-  </si>
-  <si>
-    <t>Suggest some sci-fi movies</t>
+    <t>Could you recommend some horror films to me?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to watch a horror movie. Any recommendations? </t>
+  </si>
+  <si>
+    <t>I would like to watch a horror film</t>
+  </si>
+  <si>
+    <t>List some popular horror movies</t>
+  </si>
+  <si>
+    <t>Suggest some horror movies</t>
+  </si>
+  <si>
+    <t>Recommend me some comedies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to see some comedies </t>
+  </si>
+  <si>
+    <t>Recommend me some horror films</t>
+  </si>
+  <si>
+    <t>Recommend me some horror movies</t>
+  </si>
+  <si>
+    <t>I would like to watch some funny films</t>
+  </si>
+  <si>
+    <t>I would like to watch some funny movies</t>
+  </si>
+  <si>
+    <t>I want to see a horror movie</t>
+  </si>
+  <si>
+    <t>I want to see a horror movies</t>
+  </si>
+  <si>
+    <t>I want to see some horror films</t>
   </si>
   <si>
     <t>What to watch recently</t>
@@ -376,13 +403,16 @@
     <t>Are there any new comedies recently</t>
   </si>
   <si>
-    <t>Are there any comedies on show</t>
+    <t>Are there any comedies on show now</t>
   </si>
   <si>
     <t>What movie will be released</t>
   </si>
   <si>
-    <t>I would like to see some on show movies</t>
+    <t>Recommend some movies are on show now</t>
+  </si>
+  <si>
+    <t>I want to see some films that are on show now</t>
   </si>
   <si>
     <t>I want to see some comedies in cinema</t>
@@ -394,31 +424,40 @@
     <t>I would like to see some new comedies</t>
   </si>
   <si>
-    <t>Will any happy movies be on recently</t>
+    <t>Will any horror movies be on recently</t>
   </si>
   <si>
     <t>Recommend me some upcoming horror films</t>
   </si>
   <si>
-    <t>Will any romantic movies be in the theatre recently</t>
-  </si>
-  <si>
-    <t>Will any action movies be released recently</t>
+    <t>Will any horror movies be in the theatre recently</t>
+  </si>
+  <si>
+    <t>Will any horror movies be released recently</t>
   </si>
   <si>
     <t>I would like to watch some new funny films</t>
   </si>
   <si>
-    <t>I want to see a new released adventure movie</t>
-  </si>
-  <si>
-    <t>Are there any action movies on show now?</t>
-  </si>
-  <si>
-    <t>I want to see some happy films in cinema</t>
-  </si>
-  <si>
-    <t>Are there any new adventure movies now?</t>
+    <t>I want to see a new released horror movie</t>
+  </si>
+  <si>
+    <t>Are there any horror movies on show now</t>
+  </si>
+  <si>
+    <t>I want to see some horror films in cinema</t>
+  </si>
+  <si>
+    <t>Are there any new horror movies now</t>
+  </si>
+  <si>
+    <t>Are there any horror movies in the cinemas now</t>
+  </si>
+  <si>
+    <t>Any new comedies recently</t>
+  </si>
+  <si>
+    <t>Any new horror movies recently</t>
   </si>
   <si>
     <t>How is the storyline of Joker.</t>
@@ -485,6 +524,30 @@
   </si>
   <si>
     <t>Is the story good in Joker</t>
+  </si>
+  <si>
+    <t>How is the actors in Joker</t>
+  </si>
+  <si>
+    <t>How is the actors of Joker</t>
+  </si>
+  <si>
+    <t>How is the performance of actors in Joker</t>
+  </si>
+  <si>
+    <t>How is the actor of Joker</t>
+  </si>
+  <si>
+    <t>How is the sound effects of Joker</t>
+  </si>
+  <si>
+    <t>How is the sound of Joker</t>
+  </si>
+  <si>
+    <t>How is the visual effects of Joker</t>
+  </si>
+  <si>
+    <t>How is the director of Joker</t>
   </si>
   <si>
     <t>What is other audiences think of Joker</t>
@@ -563,7 +626,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -578,6 +641,11 @@
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="14"/>
@@ -665,7 +733,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -693,7 +761,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1782,7 +1853,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E222"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2787,7 +2858,7 @@
     </row>
     <row r="95" ht="13.65" customHeight="1">
       <c r="A95" t="s" s="2">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s" s="2">
         <v>89</v>
@@ -2798,7 +2869,7 @@
     </row>
     <row r="96" ht="13.65" customHeight="1">
       <c r="A96" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s" s="2">
         <v>89</v>
@@ -2809,7 +2880,7 @@
     </row>
     <row r="97" ht="13.65" customHeight="1">
       <c r="A97" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s" s="2">
         <v>89</v>
@@ -2820,7 +2891,7 @@
     </row>
     <row r="98" ht="13.65" customHeight="1">
       <c r="A98" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s" s="2">
         <v>89</v>
@@ -2831,7 +2902,7 @@
     </row>
     <row r="99" ht="13.65" customHeight="1">
       <c r="A99" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s" s="2">
         <v>89</v>
@@ -2842,7 +2913,7 @@
     </row>
     <row r="100" ht="13.65" customHeight="1">
       <c r="A100" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s" s="2">
         <v>89</v>
@@ -2853,7 +2924,7 @@
     </row>
     <row r="101" ht="13.65" customHeight="1">
       <c r="A101" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s" s="2">
         <v>89</v>
@@ -2864,7 +2935,7 @@
     </row>
     <row r="102" ht="13.65" customHeight="1">
       <c r="A102" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s" s="2">
         <v>89</v>
@@ -2875,7 +2946,7 @@
     </row>
     <row r="103" ht="13.65" customHeight="1">
       <c r="A103" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s" s="2">
         <v>89</v>
@@ -2886,7 +2957,7 @@
     </row>
     <row r="104" ht="13.65" customHeight="1">
       <c r="A104" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s" s="2">
         <v>89</v>
@@ -2897,7 +2968,7 @@
     </row>
     <row r="105" ht="13.65" customHeight="1">
       <c r="A105" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s" s="2">
         <v>89</v>
@@ -2908,7 +2979,7 @@
     </row>
     <row r="106" ht="13.65" customHeight="1">
       <c r="A106" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s" s="2">
         <v>89</v>
@@ -2918,128 +2989,128 @@
       <c r="E106" s="3"/>
     </row>
     <row r="107" ht="13.65" customHeight="1">
-      <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
+      <c r="A107" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s" s="2">
+        <v>89</v>
+      </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
     </row>
     <row r="108" ht="13.65" customHeight="1">
       <c r="A108" t="s" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
     </row>
     <row r="109" ht="13.65" customHeight="1">
-      <c r="A109" t="s" s="4">
-        <v>106</v>
+      <c r="A109" t="s" s="2">
+        <v>107</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
     </row>
     <row r="110" ht="13.65" customHeight="1">
-      <c r="A110" t="s" s="5">
-        <v>107</v>
+      <c r="A110" t="s" s="2">
+        <v>108</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
     </row>
     <row r="111" ht="13.65" customHeight="1">
-      <c r="A111" t="s" s="5">
-        <v>108</v>
+      <c r="A111" t="s" s="2">
+        <v>109</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
     </row>
     <row r="112" ht="13.65" customHeight="1">
-      <c r="A112" t="s" s="5">
-        <v>109</v>
+      <c r="A112" t="s" s="2">
+        <v>110</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
     </row>
     <row r="113" ht="13.65" customHeight="1">
-      <c r="A113" t="s" s="5">
-        <v>110</v>
+      <c r="A113" t="s" s="2">
+        <v>111</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
     </row>
     <row r="114" ht="13.65" customHeight="1">
-      <c r="A114" t="s" s="5">
-        <v>111</v>
+      <c r="A114" t="s" s="2">
+        <v>112</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
     </row>
     <row r="115" ht="13.65" customHeight="1">
-      <c r="A115" t="s" s="5">
-        <v>112</v>
-      </c>
-      <c r="B115" t="s" s="2">
-        <v>105</v>
-      </c>
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
     </row>
     <row r="116" ht="13.65" customHeight="1">
-      <c r="A116" t="s" s="5">
+      <c r="A116" t="s" s="2">
         <v>113</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
     </row>
     <row r="117" ht="13.65" customHeight="1">
-      <c r="A117" t="s" s="5">
+      <c r="A117" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="B117" t="s" s="2">
-        <v>105</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
     </row>
     <row r="118" ht="13.65" customHeight="1">
-      <c r="A118" t="s" s="5">
-        <v>115</v>
+      <c r="A118" t="s" s="4">
+        <v>116</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
@@ -3047,10 +3118,10 @@
     </row>
     <row r="119" ht="13.65" customHeight="1">
       <c r="A119" t="s" s="5">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B119" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
@@ -3058,10 +3129,10 @@
     </row>
     <row r="120" ht="13.65" customHeight="1">
       <c r="A120" t="s" s="5">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
@@ -3069,10 +3140,10 @@
     </row>
     <row r="121" ht="13.65" customHeight="1">
       <c r="A121" t="s" s="5">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
@@ -3080,10 +3151,10 @@
     </row>
     <row r="122" ht="13.65" customHeight="1">
       <c r="A122" t="s" s="5">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
@@ -3091,10 +3162,10 @@
     </row>
     <row r="123" ht="13.65" customHeight="1">
       <c r="A123" t="s" s="5">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
@@ -3102,10 +3173,10 @@
     </row>
     <row r="124" ht="13.65" customHeight="1">
       <c r="A124" t="s" s="5">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
@@ -3113,10 +3184,10 @@
     </row>
     <row r="125" ht="13.65" customHeight="1">
       <c r="A125" t="s" s="5">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
@@ -3124,10 +3195,10 @@
     </row>
     <row r="126" ht="13.65" customHeight="1">
       <c r="A126" t="s" s="5">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
@@ -3135,10 +3206,10 @@
     </row>
     <row r="127" ht="13.65" customHeight="1">
       <c r="A127" t="s" s="5">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
@@ -3146,10 +3217,10 @@
     </row>
     <row r="128" ht="13.65" customHeight="1">
       <c r="A128" t="s" s="5">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
@@ -3157,10 +3228,10 @@
     </row>
     <row r="129" ht="13.65" customHeight="1">
       <c r="A129" t="s" s="5">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
@@ -3168,10 +3239,10 @@
     </row>
     <row r="130" ht="13.65" customHeight="1">
       <c r="A130" t="s" s="5">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
@@ -3179,10 +3250,10 @@
     </row>
     <row r="131" ht="13.65" customHeight="1">
       <c r="A131" t="s" s="5">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B131" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
@@ -3190,10 +3261,10 @@
     </row>
     <row r="132" ht="13.65" customHeight="1">
       <c r="A132" t="s" s="5">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
@@ -3201,10 +3272,10 @@
     </row>
     <row r="133" ht="13.65" customHeight="1">
       <c r="A133" t="s" s="5">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
@@ -3215,7 +3286,7 @@
         <v>131</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
@@ -3226,7 +3297,7 @@
         <v>132</v>
       </c>
       <c r="B135" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
@@ -3237,7 +3308,7 @@
         <v>133</v>
       </c>
       <c r="B136" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
@@ -3248,7 +3319,7 @@
         <v>134</v>
       </c>
       <c r="B137" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
@@ -3259,25 +3330,29 @@
         <v>135</v>
       </c>
       <c r="B138" t="s" s="2">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
     </row>
     <row r="139" ht="13.65" customHeight="1">
-      <c r="A139" s="6"/>
-      <c r="B139" s="3"/>
+      <c r="A139" t="s" s="5">
+        <v>136</v>
+      </c>
+      <c r="B139" t="s" s="2">
+        <v>114</v>
+      </c>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
     </row>
     <row r="140" ht="13.65" customHeight="1">
       <c r="A140" t="s" s="5">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B140" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
@@ -3288,7 +3363,7 @@
         <v>138</v>
       </c>
       <c r="B141" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
@@ -3299,7 +3374,7 @@
         <v>139</v>
       </c>
       <c r="B142" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
@@ -3310,7 +3385,7 @@
         <v>140</v>
       </c>
       <c r="B143" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
@@ -3321,7 +3396,7 @@
         <v>141</v>
       </c>
       <c r="B144" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -3332,7 +3407,7 @@
         <v>142</v>
       </c>
       <c r="B145" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
@@ -3343,7 +3418,7 @@
         <v>143</v>
       </c>
       <c r="B146" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
@@ -3354,7 +3429,7 @@
         <v>144</v>
       </c>
       <c r="B147" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
@@ -3365,7 +3440,7 @@
         <v>145</v>
       </c>
       <c r="B148" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
@@ -3376,7 +3451,7 @@
         <v>146</v>
       </c>
       <c r="B149" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
@@ -3387,7 +3462,7 @@
         <v>147</v>
       </c>
       <c r="B150" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
@@ -3398,29 +3473,25 @@
         <v>148</v>
       </c>
       <c r="B151" t="s" s="2">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
     </row>
     <row r="152" ht="13.65" customHeight="1">
-      <c r="A152" t="s" s="5">
-        <v>149</v>
-      </c>
-      <c r="B152" t="s" s="2">
-        <v>137</v>
-      </c>
+      <c r="A152" s="6"/>
+      <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
     </row>
     <row r="153" ht="13.65" customHeight="1">
       <c r="A153" t="s" s="5">
+        <v>149</v>
+      </c>
+      <c r="B153" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="B153" t="s" s="2">
-        <v>137</v>
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
@@ -3431,7 +3502,7 @@
         <v>151</v>
       </c>
       <c r="B154" t="s" s="2">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
@@ -3442,7 +3513,7 @@
         <v>152</v>
       </c>
       <c r="B155" t="s" s="2">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
@@ -3453,7 +3524,7 @@
         <v>153</v>
       </c>
       <c r="B156" t="s" s="2">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
@@ -3464,7 +3535,7 @@
         <v>154</v>
       </c>
       <c r="B157" t="s" s="2">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
@@ -3475,7 +3546,7 @@
         <v>155</v>
       </c>
       <c r="B158" t="s" s="2">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
@@ -3486,38 +3557,42 @@
         <v>156</v>
       </c>
       <c r="B159" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="C159" s="7"/>
+        <v>150</v>
+      </c>
+      <c r="C159" s="3"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
     </row>
     <row r="160" ht="13.65" customHeight="1">
-      <c r="A160" t="s" s="8">
+      <c r="A160" t="s" s="5">
         <v>157</v>
       </c>
       <c r="B160" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="C160" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C160" s="3"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
     </row>
     <row r="161" ht="13.65" customHeight="1">
-      <c r="A161" s="9"/>
-      <c r="B161" s="3"/>
-      <c r="C161" s="6"/>
+      <c r="A161" t="s" s="5">
+        <v>158</v>
+      </c>
+      <c r="B161" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="C161" s="3"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
     </row>
     <row r="162" ht="13.65" customHeight="1">
       <c r="A162" t="s" s="5">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B162" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C162" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C162" s="3"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
     </row>
@@ -3526,20 +3601,20 @@
         <v>160</v>
       </c>
       <c r="B163" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C163" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C163" s="3"/>
       <c r="D163" s="3"/>
       <c r="E163" s="3"/>
     </row>
     <row r="164" ht="13.65" customHeight="1">
-      <c r="A164" t="s" s="8">
+      <c r="A164" t="s" s="5">
         <v>161</v>
       </c>
       <c r="B164" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C164" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C164" s="3"/>
       <c r="D164" s="3"/>
       <c r="E164" s="3"/>
     </row>
@@ -3548,20 +3623,20 @@
         <v>162</v>
       </c>
       <c r="B165" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C165" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C165" s="3"/>
       <c r="D165" s="3"/>
       <c r="E165" s="3"/>
     </row>
     <row r="166" ht="13.65" customHeight="1">
-      <c r="A166" t="s" s="8">
+      <c r="A166" t="s" s="5">
         <v>163</v>
       </c>
       <c r="B166" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C166" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C166" s="3"/>
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
     </row>
@@ -3570,20 +3645,20 @@
         <v>164</v>
       </c>
       <c r="B167" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C167" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C167" s="3"/>
       <c r="D167" s="3"/>
       <c r="E167" s="3"/>
     </row>
     <row r="168" ht="13.65" customHeight="1">
-      <c r="A168" t="s" s="8">
+      <c r="A168" t="s" s="5">
         <v>165</v>
       </c>
       <c r="B168" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C168" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C168" s="3"/>
       <c r="D168" s="3"/>
       <c r="E168" s="3"/>
     </row>
@@ -3592,214 +3667,246 @@
         <v>166</v>
       </c>
       <c r="B169" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C169" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C169" s="3"/>
       <c r="D169" s="3"/>
       <c r="E169" s="3"/>
     </row>
     <row r="170" ht="13.65" customHeight="1">
-      <c r="A170" t="s" s="8">
+      <c r="A170" t="s" s="5">
         <v>167</v>
       </c>
       <c r="B170" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="C170" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="3"/>
     </row>
     <row r="171" ht="13.65" customHeight="1">
-      <c r="A171" s="6"/>
-      <c r="B171" s="3"/>
-      <c r="C171" s="6"/>
+      <c r="A171" t="s" s="5">
+        <v>168</v>
+      </c>
+      <c r="B171" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="C171" s="3"/>
       <c r="D171" s="3"/>
       <c r="E171" s="3"/>
     </row>
     <row r="172" ht="13.65" customHeight="1">
-      <c r="A172" t="s" s="8">
-        <v>168</v>
+      <c r="A172" t="s" s="5">
+        <v>169</v>
       </c>
       <c r="B172" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="C172" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C172" s="7"/>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
     </row>
     <row r="173" ht="13.65" customHeight="1">
-      <c r="A173" t="s" s="5">
+      <c r="A173" t="s" s="8">
         <v>170</v>
       </c>
       <c r="B173" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C173" s="6"/>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
     </row>
     <row r="174" ht="13.65" customHeight="1">
-      <c r="A174" t="s" s="8">
+      <c r="A174" t="s" s="9">
         <v>171</v>
       </c>
       <c r="B174" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C174" s="6"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
     </row>
     <row r="175" ht="13.65" customHeight="1">
-      <c r="A175" t="s" s="5">
+      <c r="A175" t="s" s="9">
         <v>172</v>
       </c>
       <c r="B175" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C175" s="6"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
     </row>
     <row r="176" ht="13.65" customHeight="1">
-      <c r="A176" t="s" s="8">
+      <c r="A176" t="s" s="9">
         <v>173</v>
       </c>
       <c r="B176" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C176" s="6"/>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
     </row>
     <row r="177" ht="13.65" customHeight="1">
-      <c r="A177" t="s" s="5">
+      <c r="A177" t="s" s="9">
         <v>174</v>
       </c>
       <c r="B177" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C177" s="6"/>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
     </row>
     <row r="178" ht="13.65" customHeight="1">
-      <c r="A178" t="s" s="8">
+      <c r="A178" t="s" s="9">
         <v>175</v>
       </c>
       <c r="B178" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C178" s="6"/>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
     </row>
     <row r="179" ht="13.65" customHeight="1">
-      <c r="A179" t="s" s="5">
+      <c r="A179" t="s" s="9">
         <v>176</v>
       </c>
       <c r="B179" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C179" s="6"/>
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
     </row>
     <row r="180" ht="13.65" customHeight="1">
-      <c r="A180" t="s" s="5">
+      <c r="A180" t="s" s="9">
         <v>177</v>
       </c>
       <c r="B180" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C180" s="6"/>
       <c r="D180" s="3"/>
       <c r="E180" s="3"/>
     </row>
     <row r="181" ht="13.65" customHeight="1">
-      <c r="A181" t="s" s="5">
+      <c r="A181" t="s" s="9">
         <v>178</v>
       </c>
       <c r="B181" t="s" s="2">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C181" s="6"/>
       <c r="D181" s="3"/>
       <c r="E181" s="3"/>
     </row>
     <row r="182" ht="13.65" customHeight="1">
-      <c r="A182" t="s" s="5">
-        <v>179</v>
-      </c>
-      <c r="B182" t="s" s="2">
-        <v>169</v>
-      </c>
+      <c r="A182" s="10"/>
+      <c r="B182" s="3"/>
       <c r="C182" s="6"/>
       <c r="D182" s="3"/>
       <c r="E182" s="3"/>
     </row>
     <row r="183" ht="13.65" customHeight="1">
       <c r="A183" t="s" s="5">
+        <v>179</v>
+      </c>
+      <c r="B183" t="s" s="2">
         <v>180</v>
-      </c>
-      <c r="B183" t="s" s="2">
-        <v>169</v>
       </c>
       <c r="C183" s="6"/>
       <c r="D183" s="3"/>
       <c r="E183" s="3"/>
     </row>
     <row r="184" ht="13.65" customHeight="1">
-      <c r="A184" s="6"/>
-      <c r="B184" s="3"/>
+      <c r="A184" t="s" s="5">
+        <v>181</v>
+      </c>
+      <c r="B184" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C184" s="6"/>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
     </row>
     <row r="185" ht="13.65" customHeight="1">
-      <c r="A185" s="6"/>
-      <c r="B185" s="3"/>
+      <c r="A185" t="s" s="8">
+        <v>182</v>
+      </c>
+      <c r="B185" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C185" s="6"/>
       <c r="D185" s="3"/>
       <c r="E185" s="3"/>
     </row>
     <row r="186" ht="13.65" customHeight="1">
-      <c r="A186" s="6"/>
-      <c r="B186" s="3"/>
+      <c r="A186" t="s" s="5">
+        <v>183</v>
+      </c>
+      <c r="B186" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C186" s="6"/>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
     </row>
     <row r="187" ht="13.65" customHeight="1">
-      <c r="A187" s="6"/>
-      <c r="B187" s="3"/>
+      <c r="A187" t="s" s="8">
+        <v>184</v>
+      </c>
+      <c r="B187" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C187" s="6"/>
       <c r="D187" s="3"/>
       <c r="E187" s="3"/>
     </row>
     <row r="188" ht="13.65" customHeight="1">
-      <c r="A188" s="6"/>
-      <c r="B188" s="3"/>
+      <c r="A188" t="s" s="5">
+        <v>185</v>
+      </c>
+      <c r="B188" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C188" s="6"/>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
     </row>
     <row r="189" ht="13.65" customHeight="1">
-      <c r="A189" s="6"/>
-      <c r="B189" s="3"/>
+      <c r="A189" t="s" s="8">
+        <v>186</v>
+      </c>
+      <c r="B189" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C189" s="6"/>
       <c r="D189" s="3"/>
       <c r="E189" s="3"/>
     </row>
     <row r="190" ht="13.65" customHeight="1">
-      <c r="A190" s="6"/>
-      <c r="B190" s="3"/>
+      <c r="A190" t="s" s="5">
+        <v>187</v>
+      </c>
+      <c r="B190" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C190" s="6"/>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
     </row>
     <row r="191" ht="13.65" customHeight="1">
-      <c r="A191" s="6"/>
-      <c r="B191" s="3"/>
+      <c r="A191" t="s" s="8">
+        <v>188</v>
+      </c>
+      <c r="B191" t="s" s="2">
+        <v>180</v>
+      </c>
       <c r="C191" s="6"/>
       <c r="D191" s="3"/>
       <c r="E191" s="3"/>
@@ -3812,67 +3919,262 @@
       <c r="E192" s="3"/>
     </row>
     <row r="193" ht="13.65" customHeight="1">
-      <c r="A193" s="6"/>
-      <c r="B193" s="3"/>
+      <c r="A193" t="s" s="8">
+        <v>189</v>
+      </c>
+      <c r="B193" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C193" s="6"/>
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
     </row>
     <row r="194" ht="13.65" customHeight="1">
-      <c r="A194" s="6"/>
-      <c r="B194" s="3"/>
+      <c r="A194" t="s" s="5">
+        <v>191</v>
+      </c>
+      <c r="B194" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C194" s="6"/>
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
     </row>
     <row r="195" ht="13.65" customHeight="1">
-      <c r="A195" s="6"/>
-      <c r="B195" s="3"/>
+      <c r="A195" t="s" s="8">
+        <v>192</v>
+      </c>
+      <c r="B195" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C195" s="6"/>
       <c r="D195" s="3"/>
       <c r="E195" s="3"/>
     </row>
     <row r="196" ht="13.65" customHeight="1">
-      <c r="A196" s="6"/>
-      <c r="B196" s="3"/>
+      <c r="A196" t="s" s="5">
+        <v>193</v>
+      </c>
+      <c r="B196" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C196" s="6"/>
       <c r="D196" s="3"/>
       <c r="E196" s="3"/>
     </row>
     <row r="197" ht="13.65" customHeight="1">
-      <c r="A197" s="6"/>
-      <c r="B197" s="3"/>
+      <c r="A197" t="s" s="8">
+        <v>194</v>
+      </c>
+      <c r="B197" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C197" s="6"/>
       <c r="D197" s="3"/>
       <c r="E197" s="3"/>
     </row>
     <row r="198" ht="13.65" customHeight="1">
-      <c r="A198" s="6"/>
-      <c r="B198" s="3"/>
+      <c r="A198" t="s" s="5">
+        <v>195</v>
+      </c>
+      <c r="B198" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C198" s="6"/>
       <c r="D198" s="3"/>
       <c r="E198" s="3"/>
     </row>
     <row r="199" ht="13.65" customHeight="1">
-      <c r="A199" s="6"/>
-      <c r="B199" s="3"/>
+      <c r="A199" t="s" s="8">
+        <v>196</v>
+      </c>
+      <c r="B199" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C199" s="6"/>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
     </row>
     <row r="200" ht="13.65" customHeight="1">
-      <c r="A200" s="6"/>
-      <c r="B200" s="3"/>
+      <c r="A200" t="s" s="5">
+        <v>197</v>
+      </c>
+      <c r="B200" t="s" s="2">
+        <v>190</v>
+      </c>
       <c r="C200" s="6"/>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
     </row>
     <row r="201" ht="13.65" customHeight="1">
-      <c r="A201" s="10"/>
-      <c r="B201" s="3"/>
-      <c r="C201" s="10"/>
+      <c r="A201" t="s" s="5">
+        <v>198</v>
+      </c>
+      <c r="B201" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="C201" s="6"/>
       <c r="D201" s="3"/>
       <c r="E201" s="3"/>
+    </row>
+    <row r="202" ht="13.65" customHeight="1">
+      <c r="A202" t="s" s="5">
+        <v>199</v>
+      </c>
+      <c r="B202" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="C202" s="6"/>
+      <c r="D202" s="3"/>
+      <c r="E202" s="3"/>
+    </row>
+    <row r="203" ht="13.65" customHeight="1">
+      <c r="A203" t="s" s="5">
+        <v>200</v>
+      </c>
+      <c r="B203" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="C203" s="6"/>
+      <c r="D203" s="3"/>
+      <c r="E203" s="3"/>
+    </row>
+    <row r="204" ht="13.65" customHeight="1">
+      <c r="A204" t="s" s="5">
+        <v>201</v>
+      </c>
+      <c r="B204" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="C204" s="6"/>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3"/>
+    </row>
+    <row r="205" ht="13.65" customHeight="1">
+      <c r="A205" s="6"/>
+      <c r="B205" s="3"/>
+      <c r="C205" s="6"/>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3"/>
+    </row>
+    <row r="206" ht="13.65" customHeight="1">
+      <c r="A206" s="6"/>
+      <c r="B206" s="3"/>
+      <c r="C206" s="6"/>
+      <c r="D206" s="3"/>
+      <c r="E206" s="3"/>
+    </row>
+    <row r="207" ht="13.65" customHeight="1">
+      <c r="A207" s="6"/>
+      <c r="B207" s="3"/>
+      <c r="C207" s="6"/>
+      <c r="D207" s="3"/>
+      <c r="E207" s="3"/>
+    </row>
+    <row r="208" ht="13.65" customHeight="1">
+      <c r="A208" s="6"/>
+      <c r="B208" s="3"/>
+      <c r="C208" s="6"/>
+      <c r="D208" s="3"/>
+      <c r="E208" s="3"/>
+    </row>
+    <row r="209" ht="13.65" customHeight="1">
+      <c r="A209" s="6"/>
+      <c r="B209" s="3"/>
+      <c r="C209" s="6"/>
+      <c r="D209" s="3"/>
+      <c r="E209" s="3"/>
+    </row>
+    <row r="210" ht="13.65" customHeight="1">
+      <c r="A210" s="6"/>
+      <c r="B210" s="3"/>
+      <c r="C210" s="6"/>
+      <c r="D210" s="3"/>
+      <c r="E210" s="3"/>
+    </row>
+    <row r="211" ht="13.65" customHeight="1">
+      <c r="A211" s="6"/>
+      <c r="B211" s="3"/>
+      <c r="C211" s="6"/>
+      <c r="D211" s="3"/>
+      <c r="E211" s="3"/>
+    </row>
+    <row r="212" ht="13.65" customHeight="1">
+      <c r="A212" s="6"/>
+      <c r="B212" s="3"/>
+      <c r="C212" s="6"/>
+      <c r="D212" s="3"/>
+      <c r="E212" s="3"/>
+    </row>
+    <row r="213" ht="13.65" customHeight="1">
+      <c r="A213" s="6"/>
+      <c r="B213" s="3"/>
+      <c r="C213" s="6"/>
+      <c r="D213" s="3"/>
+      <c r="E213" s="3"/>
+    </row>
+    <row r="214" ht="13.65" customHeight="1">
+      <c r="A214" s="6"/>
+      <c r="B214" s="3"/>
+      <c r="C214" s="6"/>
+      <c r="D214" s="3"/>
+      <c r="E214" s="3"/>
+    </row>
+    <row r="215" ht="13.65" customHeight="1">
+      <c r="A215" s="6"/>
+      <c r="B215" s="3"/>
+      <c r="C215" s="6"/>
+      <c r="D215" s="3"/>
+      <c r="E215" s="3"/>
+    </row>
+    <row r="216" ht="13.65" customHeight="1">
+      <c r="A216" s="6"/>
+      <c r="B216" s="3"/>
+      <c r="C216" s="6"/>
+      <c r="D216" s="3"/>
+      <c r="E216" s="3"/>
+    </row>
+    <row r="217" ht="13.65" customHeight="1">
+      <c r="A217" s="6"/>
+      <c r="B217" s="3"/>
+      <c r="C217" s="6"/>
+      <c r="D217" s="3"/>
+      <c r="E217" s="3"/>
+    </row>
+    <row r="218" ht="13.65" customHeight="1">
+      <c r="A218" s="6"/>
+      <c r="B218" s="3"/>
+      <c r="C218" s="6"/>
+      <c r="D218" s="3"/>
+      <c r="E218" s="3"/>
+    </row>
+    <row r="219" ht="13.65" customHeight="1">
+      <c r="A219" s="6"/>
+      <c r="B219" s="3"/>
+      <c r="C219" s="6"/>
+      <c r="D219" s="3"/>
+      <c r="E219" s="3"/>
+    </row>
+    <row r="220" ht="13.65" customHeight="1">
+      <c r="A220" s="6"/>
+      <c r="B220" s="3"/>
+      <c r="C220" s="6"/>
+      <c r="D220" s="3"/>
+      <c r="E220" s="3"/>
+    </row>
+    <row r="221" ht="13.65" customHeight="1">
+      <c r="A221" s="6"/>
+      <c r="B221" s="3"/>
+      <c r="C221" s="6"/>
+      <c r="D221" s="3"/>
+      <c r="E221" s="3"/>
+    </row>
+    <row r="222" ht="13.65" customHeight="1">
+      <c r="A222" s="11"/>
+      <c r="B222" s="3"/>
+      <c r="C222" s="11"/>
+      <c r="D222" s="3"/>
+      <c r="E222" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>